<commit_message>
Adding some questions regarading the CYRS document in the SIQ doucment Signed-off-by: MostafaNader96 <mnader96@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Abdelrahman\project\Input documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <definedNames>
+    <definedName name="_Toc30617783" localSheetId="0">Sheet1!$A$2</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Reqirement_ID</t>
   </si>
@@ -41,21 +52,75 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Req_ PO3_DGW_CYRS_02_V01</t>
+  </si>
+  <si>
+    <t>23/01/2020</t>
+  </si>
+  <si>
+    <t>Question in the alarm part</t>
+  </si>
+  <si>
+    <t>what is the time ultil the alarm stops?</t>
+  </si>
+  <si>
+    <t>what is the tone of the alarm buzzer</t>
+  </si>
+  <si>
+    <t>Req_ PO3_DGW_CYRS_06_V01</t>
+  </si>
+  <si>
+    <t>Question regarding the buttons</t>
+  </si>
+  <si>
+    <t>What is the action that happens when each of the 3 buttons are pressed in each mode?</t>
+  </si>
+  <si>
+    <t>Does each click on the buttons makes sound from the buzzer?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -63,7 +128,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -73,32 +138,50 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -288,31 +371,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.86"/>
-    <col customWidth="1" min="2" max="2" width="19.43"/>
-    <col customWidth="1" min="3" max="3" width="19.0"/>
-    <col customWidth="1" min="4" max="4" width="17.29"/>
-    <col customWidth="1" min="5" max="5" width="22.57"/>
-    <col customWidth="1" min="6" max="6" width="16.0"/>
-    <col customWidth="1" min="7" max="7" width="17.29"/>
-    <col customWidth="1" min="8" max="8" width="15.86"/>
-    <col customWidth="1" min="9" max="9" width="20.57"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="62.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -344,7 +432,76 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Review sheets for (HSI, CYRS), Update SIQ sheet
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti data\software engineering\Project\Folder_Structure\Input documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsharaby\Documents\GitHub\DWTCH_Norhan\Input documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Reqirement_ID</t>
   </si>
@@ -79,6 +79,26 @@
   </si>
   <si>
     <t>Does each click on the buttons makes sound from the buzzer?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH: 24/01/2020 : The Alarm stop when press stop or 1 min passes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH: 24/01/2020 : The normal tone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH: 24/1/2020 : You can use the 3 buttons as follows:
+For Watch and Alarms modes 
+1- Button 1: Mode change "Watch , Alarm , stop watch"
+2-Button 2 : Adjust/Select for hours minutes 
+3- Button 3 : Up increment to set the hours or minutes
+For Stop watch the change in :
+- Button 2 : will be used to start and pause the stop watch 
+- Button 3 : used to reset the stop watch 
+You can off the alarm by Up increment if the alarm is on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH: 24/01/2020 : no just for the alarm </t>
   </si>
 </sst>
 </file>
@@ -149,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -163,6 +183,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,8 +406,8 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -397,7 +420,7 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="20.5546875" customWidth="1"/>
+    <col min="9" max="9" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
@@ -448,6 +471,9 @@
       <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -465,8 +491,11 @@
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -481,6 +510,9 @@
       </c>
       <c r="F4" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -498,6 +530,9 @@
       </c>
       <c r="F5" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reformatting CYRS,HSI,SRS Documents & Updatting RTM
Signed-off-by: NorhanNassar <norhan.nassar96@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ.xlsx
+++ b/Input documents/SIQ.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsharaby\Documents\GitHub\DWTCH_Norhan\Input documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti data\software engineering\Folder_Structure\Input documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="2940" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Reqirement_ID</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Answer</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>Req_ PO3_DGW_CYRS_02_V01</t>
@@ -143,7 +140,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +150,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -169,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,6 +188,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,8 +412,8 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -451,88 +457,86 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>